<commit_message>
T1: 100b for each type finished and refactored
</commit_message>
<xml_diff>
--- a/Fizyka_Sprawka/FinalPrinted.xlsx
+++ b/Fizyka_Sprawka/FinalPrinted.xlsx
@@ -209,9 +209,6 @@
     <t>b) Wyznacz średnią wartość zmierzonej średnicy przedmiotu. Obliczyć jej niepewność pomiarową, Tuleja</t>
   </si>
   <si>
-    <t>Tuleja Zew</t>
-  </si>
-  <si>
     <t>Całkowita Niep. Stand.- Obliczenie - Zew</t>
   </si>
   <si>
@@ -221,10 +218,13 @@
     <t>Całkowita Niep. Stand.- Obliczenie - Wys</t>
   </si>
   <si>
-    <t>Tuleja Wew</t>
+    <t>Całkowita Niep. Stand.- Obliczenie - Wew</t>
   </si>
   <si>
-    <t>Całkowita Niep. Stand.- Obliczenie - Wew</t>
+    <t>Tuleja Średnica Wew</t>
+  </si>
+  <si>
+    <t>Tuleja Średnica Zew</t>
   </si>
 </sst>
 </file>
@@ -232,8 +232,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
-    <numFmt numFmtId="168" formatCode="#,##0.0000000000"/>
-    <numFmt numFmtId="169" formatCode="0.000000"/>
+    <numFmt numFmtId="164" formatCode="#,##0.0000000000"/>
+    <numFmt numFmtId="165" formatCode="0.000000"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -280,30 +280,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -873,7 +855,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="151">
+  <cellXfs count="134">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -897,43 +879,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
@@ -959,191 +905,63 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="168" fontId="0" fillId="5" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1"/>
@@ -1157,20 +975,155 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1198,8 +1151,8 @@
       <xdr:rowOff>188844</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="298287" cy="354841"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="TextBox 1"/>
@@ -1315,7 +1268,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="TextBox 1"/>
@@ -1402,8 +1355,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="298287" cy="182217"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3" name="TextBox 2"/>
@@ -1519,7 +1472,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3" name="TextBox 2"/>
@@ -1606,8 +1559,8 @@
       <xdr:rowOff>41284</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1748116" cy="486514"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="4" name="TextBox 3"/>
@@ -1967,7 +1920,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="4" name="TextBox 3"/>
@@ -2250,8 +2203,8 @@
       <xdr:rowOff>2168</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2353234" cy="486514"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="5" name="TextBox 4"/>
@@ -2350,7 +2303,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="5" name="TextBox 4"/>
@@ -2420,8 +2373,8 @@
       <xdr:rowOff>134096</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1709122" cy="500137"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="6" name="TextBox 5"/>
@@ -2757,7 +2710,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="6" name="TextBox 5"/>
@@ -2895,8 +2848,8 @@
       <xdr:rowOff>33131</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="3801719" cy="776494"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="7" name="TextBox 6"/>
@@ -3622,7 +3575,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="7" name="TextBox 6"/>
@@ -3893,8 +3846,8 @@
       <xdr:rowOff>100161</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1714499" cy="486514"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="8" name="TextBox 7"/>
@@ -4130,7 +4083,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="8" name="TextBox 7"/>
@@ -4261,8 +4214,8 @@
       <xdr:rowOff>89807</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2787362" cy="1027216"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="9" name="TextBox 8"/>
@@ -4725,7 +4678,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="9" name="TextBox 8"/>
@@ -5027,8 +4980,8 @@
       <xdr:rowOff>10886</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="298287" cy="182217"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="10" name="TextBox 9"/>
@@ -5144,7 +5097,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="10" name="TextBox 9"/>
@@ -5236,8 +5189,8 @@
       <xdr:rowOff>17931</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="329453" cy="138952"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="TextBox 1"/>
@@ -5318,7 +5271,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="TextBox 1"/>
@@ -5395,8 +5348,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="298287" cy="354841"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3" name="TextBox 2"/>
@@ -5512,7 +5465,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3" name="TextBox 2"/>
@@ -5599,8 +5552,8 @@
       <xdr:rowOff>180367</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="111248" cy="172227"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="4" name="TextBox 3"/>
@@ -5669,7 +5622,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="4" name="TextBox 3"/>
@@ -5734,8 +5687,8 @@
       <xdr:rowOff>189752</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="151067" cy="172227"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="5" name="TextBox 4"/>
@@ -5811,7 +5764,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="5" name="TextBox 4"/>
@@ -5882,8 +5835,8 @@
       <xdr:rowOff>83726</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2337821" cy="602074"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="6" name="TextBox 5"/>
@@ -6369,7 +6322,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="6" name="TextBox 5"/>
@@ -6743,8 +6696,8 @@
       <xdr:rowOff>50425</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2744000" cy="890869"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="7" name="TextBox 6"/>
@@ -7452,7 +7405,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="7" name="TextBox 6"/>
@@ -7753,8 +7706,8 @@
       <xdr:rowOff>28574</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2590800" cy="885825"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="8" name="TextBox 7"/>
@@ -8306,7 +8259,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="8" name="TextBox 7"/>
@@ -8667,8 +8620,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="298287" cy="354841"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="9" name="TextBox 8"/>
@@ -8784,7 +8737,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="9" name="TextBox 8"/>
@@ -8871,8 +8824,8 @@
       <xdr:rowOff>20123</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="842015" cy="170377"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="10" name="TextBox 9"/>
@@ -8956,7 +8909,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="10" name="TextBox 9"/>
@@ -9030,8 +8983,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="298287" cy="354841"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="11" name="TextBox 10"/>
@@ -9147,7 +9100,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="11" name="TextBox 10"/>
@@ -9234,8 +9187,8 @@
       <xdr:rowOff>48698</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1020190" cy="437077"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="12" name="TextBox 11"/>
@@ -9340,7 +9293,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="12" name="TextBox 11"/>
@@ -9627,8 +9580,8 @@
       <xdr:rowOff>12887</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="266700" cy="158563"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="6" name="TextBox 5"/>
@@ -9709,7 +9662,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="6" name="TextBox 5"/>
@@ -9786,8 +9739,8 @@
       <xdr:rowOff>1190</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1104918" cy="172227"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="7" name="TextBox 6"/>
@@ -10044,7 +9997,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="7" name="TextBox 6"/>
@@ -10192,8 +10145,8 @@
       <xdr:rowOff>18742</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1146339" cy="143437"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="8" name="TextBox 7"/>
@@ -10438,7 +10391,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="8" name="TextBox 7"/>
@@ -10574,8 +10527,8 @@
       <xdr:rowOff>23446</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="929422" cy="143437"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="9" name="TextBox 8"/>
@@ -10862,7 +10815,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="9" name="TextBox 8"/>
@@ -11176,8 +11129,8 @@
       <xdr:rowOff>55978</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2433900" cy="689458"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="25" name="TextBox 24"/>
@@ -11679,7 +11632,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="25" name="TextBox 24"/>
@@ -12066,8 +12019,8 @@
       <xdr:rowOff>10717</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2575472" cy="1076254"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="26" name="TextBox 25"/>
@@ -12775,7 +12728,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="26" name="TextBox 25"/>
@@ -13076,8 +13029,8 @@
       <xdr:rowOff>17367</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2442882" cy="778250"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="27" name="TextBox 26"/>
@@ -13675,7 +13628,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="27" name="TextBox 26"/>
@@ -14094,8 +14047,8 @@
       <xdr:rowOff>55978</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2433900" cy="689458"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="28" name="TextBox 27"/>
@@ -14597,7 +14550,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="28" name="TextBox 27"/>
@@ -14984,8 +14937,8 @@
       <xdr:rowOff>10717</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2575472" cy="1076254"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="29" name="TextBox 28"/>
@@ -15693,7 +15646,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="29" name="TextBox 28"/>
@@ -15994,8 +15947,8 @@
       <xdr:rowOff>17367</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2442882" cy="778250"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="30" name="TextBox 29"/>
@@ -16578,7 +16531,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="30" name="TextBox 29"/>
@@ -17004,11 +16957,11 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>67449</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>55978</xdr:rowOff>
+      <xdr:colOff>86498</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>189328</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="2168856" cy="689458"/>
+    <xdr:ext cx="2561452" cy="572672"/>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
         <xdr:sp macro="" textlink="">
@@ -17018,8 +16971,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="2982099" y="4980403"/>
-              <a:ext cx="2168856" cy="689458"/>
+              <a:off x="86498" y="6894928"/>
+              <a:ext cx="2561452" cy="572672"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -17501,8 +17454,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="2982099" y="4980403"/>
-              <a:ext cx="2168856" cy="689458"/>
+              <a:off x="86498" y="6894928"/>
+              <a:ext cx="2561452" cy="572672"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -17857,10 +17810,10 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>64313</xdr:colOff>
-      <xdr:row>40</xdr:row>
+      <xdr:row>38</xdr:row>
       <xdr:rowOff>10717</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="2575472" cy="1076254"/>
+    <xdr:ext cx="2575472" cy="922733"/>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
         <xdr:sp macro="" textlink="">
@@ -17870,8 +17823,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="2978963" y="5906692"/>
-              <a:ext cx="2575472" cy="1076254"/>
+              <a:off x="64313" y="7859317"/>
+              <a:ext cx="2575472" cy="922733"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -18578,8 +18531,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="2978963" y="5906692"/>
-              <a:ext cx="2575472" cy="1076254"/>
+              <a:off x="64313" y="7859317"/>
+              <a:ext cx="2575472" cy="922733"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -18867,12 +18820,12 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>67235</xdr:colOff>
-      <xdr:row>47</xdr:row>
+      <xdr:row>44</xdr:row>
       <xdr:rowOff>17367</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2442882" cy="778250"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="33" name="TextBox 32"/>
@@ -19453,7 +19406,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="33" name="TextBox 32"/>
@@ -19836,23 +19789,23 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>13138</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>60763</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>190501</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="298287" cy="354841"/>
+    <xdr:ext cx="298287" cy="228600"/>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="34" name="TextBox 33"/>
+            <xdr:cNvPr id="35" name="TextBox 34"/>
             <xdr:cNvSpPr txBox="1"/>
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="2927788" y="4524375"/>
-              <a:ext cx="298287" cy="354841"/>
+              <a:off x="2708713" y="6296026"/>
+              <a:ext cx="298287" cy="228600"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -19875,7 +19828,7 @@
           </xdr:style>
           <xdr:txBody>
             <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
-              <a:spAutoFit/>
+              <a:noAutofit/>
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
@@ -19962,13 +19915,13 @@
       <mc:Fallback>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="34" name="TextBox 33"/>
+            <xdr:cNvPr id="35" name="TextBox 34"/>
             <xdr:cNvSpPr txBox="1"/>
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="2927788" y="4524375"/>
-              <a:ext cx="298287" cy="354841"/>
+              <a:off x="2708713" y="6296026"/>
+              <a:ext cx="298287" cy="228600"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -19991,7 +19944,7 @@
           </xdr:style>
           <xdr:txBody>
             <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
-              <a:spAutoFit/>
+              <a:noAutofit/>
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
@@ -20051,8 +20004,8 @@
       <xdr:rowOff>21535</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="329453" cy="138952"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="TextBox 1"/>
@@ -20133,7 +20086,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="TextBox 1"/>
@@ -20210,8 +20163,8 @@
       <xdr:rowOff>7040</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="381323" cy="172227"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3" name="TextBox 2"/>
@@ -20334,7 +20287,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3" name="TextBox 2"/>
@@ -20399,8 +20352,8 @@
       <xdr:rowOff>196298</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="387670" cy="172227"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="4" name="TextBox 3"/>
@@ -20523,7 +20476,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="4" name="TextBox 3"/>
@@ -20612,8 +20565,8 @@
       <xdr:rowOff>189257</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="381323" cy="172227"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="5" name="TextBox 4"/>
@@ -20736,7 +20689,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="5" name="TextBox 4"/>
@@ -20825,8 +20778,8 @@
       <xdr:rowOff>12010</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="329453" cy="138952"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="10" name="TextBox 9"/>
@@ -20907,7 +20860,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="10" name="TextBox 9"/>
@@ -20984,8 +20937,8 @@
       <xdr:rowOff>197540</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="381323" cy="172227"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="11" name="TextBox 10"/>
@@ -21108,7 +21061,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="11" name="TextBox 10"/>
@@ -21173,8 +21126,8 @@
       <xdr:rowOff>5798</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="387670" cy="172227"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="12" name="TextBox 11"/>
@@ -21297,7 +21250,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="12" name="TextBox 11"/>
@@ -21386,8 +21339,8 @@
       <xdr:rowOff>198782</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="381323" cy="172227"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="13" name="TextBox 12"/>
@@ -21510,7 +21463,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="13" name="TextBox 12"/>
@@ -21878,39 +21831,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="90" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="116"/>
-      <c r="J1" s="18"/>
-      <c r="K1" s="18"/>
-      <c r="L1" s="18"/>
-      <c r="M1" s="18"/>
-      <c r="N1" s="18"/>
-      <c r="O1" s="18"/>
-      <c r="P1" s="18"/>
-      <c r="Q1" s="18"/>
+      <c r="B1" s="90"/>
+      <c r="C1" s="90"/>
+      <c r="D1" s="90"/>
+      <c r="E1" s="90"/>
+      <c r="F1" s="90"/>
+      <c r="G1" s="90"/>
+      <c r="H1" s="90"/>
+      <c r="I1" s="60"/>
+      <c r="J1" s="103"/>
+      <c r="K1" s="103"/>
+      <c r="L1" s="103"/>
+      <c r="M1" s="103"/>
+      <c r="N1" s="103"/>
+      <c r="O1" s="103"/>
+      <c r="P1" s="103"/>
+      <c r="Q1" s="103"/>
     </row>
     <row r="2" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="55" t="s">
+      <c r="A2" s="83" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="57"/>
-      <c r="C2" s="57"/>
-      <c r="D2" s="56"/>
-      <c r="E2" s="13" t="s">
+      <c r="B2" s="84"/>
+      <c r="C2" s="84"/>
+      <c r="D2" s="85"/>
+      <c r="E2" s="104" t="s">
         <v>19</v>
       </c>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
+      <c r="F2" s="104"/>
+      <c r="G2" s="104"/>
+      <c r="H2" s="104"/>
     </row>
     <row r="3" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
@@ -21919,238 +21872,226 @@
       <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="55"/>
-      <c r="D3" s="56"/>
+      <c r="C3" s="83"/>
+      <c r="D3" s="85"/>
       <c r="E3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="13" t="s">
+      <c r="F3" s="104" t="s">
         <v>21</v>
       </c>
-      <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
-      <c r="K3" s="40"/>
+      <c r="G3" s="104"/>
+      <c r="H3" s="104"/>
+      <c r="K3" s="28"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="117" t="s">
+      <c r="A4" s="61" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="118">
+      <c r="B4" s="62">
         <v>0.72</v>
       </c>
-      <c r="C4" s="14"/>
-      <c r="D4" s="15"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="119" t="s">
+      <c r="C4" s="91"/>
+      <c r="D4" s="92"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="95" t="s">
         <v>22</v>
       </c>
-      <c r="G4" s="19"/>
-      <c r="H4" s="59"/>
+      <c r="G4" s="96"/>
+      <c r="H4" s="97"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5" s="120" t="s">
+      <c r="A5" s="63" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="38">
+      <c r="B5" s="26">
         <v>8.24</v>
       </c>
-      <c r="C5" s="16"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="27"/>
-      <c r="F5" s="121" t="s">
+      <c r="C5" s="93"/>
+      <c r="D5" s="94"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="98" t="s">
         <v>34</v>
       </c>
-      <c r="G5" s="21"/>
-      <c r="H5" s="61"/>
+      <c r="G5" s="87"/>
+      <c r="H5" s="88"/>
     </row>
     <row r="6" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="122" t="s">
+      <c r="A6" s="64" t="s">
         <v>35</v>
       </c>
-      <c r="B6" s="123"/>
-      <c r="C6" s="124">
+      <c r="B6" s="65"/>
+      <c r="C6" s="99">
         <v>0.01</v>
       </c>
-      <c r="D6" s="125"/>
-      <c r="E6" s="28"/>
-      <c r="F6" s="126"/>
-      <c r="G6" s="22"/>
-      <c r="H6" s="63"/>
+      <c r="D6" s="100"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="101"/>
+      <c r="G6" s="90"/>
+      <c r="H6" s="102"/>
     </row>
     <row r="7" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="55" t="s">
+      <c r="A7" s="83" t="s">
         <v>36</v>
       </c>
-      <c r="B7" s="57"/>
-      <c r="C7" s="57"/>
-      <c r="D7" s="56"/>
-      <c r="E7" s="55"/>
-      <c r="F7" s="57"/>
-      <c r="G7" s="57"/>
-      <c r="H7" s="56"/>
+      <c r="B7" s="84"/>
+      <c r="C7" s="84"/>
+      <c r="D7" s="85"/>
+      <c r="E7" s="83"/>
+      <c r="F7" s="84"/>
+      <c r="G7" s="84"/>
+      <c r="H7" s="85"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A8" s="27"/>
-      <c r="B8" s="29"/>
-      <c r="C8" s="29"/>
-      <c r="D8" s="36"/>
+      <c r="A8" s="15"/>
+      <c r="B8" s="17"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="24"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A9" s="27"/>
-      <c r="B9" s="29"/>
-      <c r="C9" s="29"/>
-      <c r="D9" s="36"/>
+      <c r="A9" s="15"/>
+      <c r="B9" s="17"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="24"/>
     </row>
     <row r="10" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="127"/>
-      <c r="B10" s="33"/>
-      <c r="C10" s="33"/>
-      <c r="D10" s="37"/>
+      <c r="A10" s="66"/>
+      <c r="B10" s="21"/>
+      <c r="C10" s="21"/>
+      <c r="D10" s="25"/>
     </row>
     <row r="11" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="55" t="s">
+      <c r="A11" s="83" t="s">
         <v>29</v>
       </c>
-      <c r="B11" s="57"/>
-      <c r="C11" s="57"/>
-      <c r="D11" s="56"/>
+      <c r="B11" s="84"/>
+      <c r="C11" s="84"/>
+      <c r="D11" s="85"/>
     </row>
     <row r="12" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="27"/>
-      <c r="B12" s="29"/>
-      <c r="C12" s="29"/>
-      <c r="D12" s="36"/>
+      <c r="A12" s="15"/>
+      <c r="B12" s="17"/>
+      <c r="C12" s="17"/>
+      <c r="D12" s="24"/>
     </row>
     <row r="13" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="55" t="s">
+      <c r="A13" s="83" t="s">
         <v>37</v>
       </c>
-      <c r="B13" s="57"/>
-      <c r="C13" s="57"/>
-      <c r="D13" s="56"/>
+      <c r="B13" s="84"/>
+      <c r="C13" s="84"/>
+      <c r="D13" s="85"/>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A14" s="60"/>
-      <c r="B14" s="21"/>
-      <c r="C14" s="21"/>
-      <c r="D14" s="61"/>
+      <c r="A14" s="86"/>
+      <c r="B14" s="87"/>
+      <c r="C14" s="87"/>
+      <c r="D14" s="88"/>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A15" s="27"/>
-      <c r="B15" s="29"/>
-      <c r="C15" s="29"/>
-      <c r="D15" s="36"/>
+      <c r="A15" s="15"/>
+      <c r="B15" s="17"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="24"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A16" s="27"/>
-      <c r="B16" s="29"/>
-      <c r="C16" s="29"/>
-      <c r="D16" s="36"/>
+      <c r="A16" s="15"/>
+      <c r="B16" s="17"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="24"/>
     </row>
     <row r="17" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="127"/>
-      <c r="B17" s="33"/>
-      <c r="C17" s="33"/>
-      <c r="D17" s="37"/>
+      <c r="A17" s="66"/>
+      <c r="B17" s="21"/>
+      <c r="C17" s="21"/>
+      <c r="D17" s="25"/>
     </row>
     <row r="18" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="55" t="s">
+      <c r="A18" s="83" t="s">
         <v>30</v>
       </c>
-      <c r="B18" s="57"/>
-      <c r="C18" s="57"/>
-      <c r="D18" s="56"/>
+      <c r="B18" s="84"/>
+      <c r="C18" s="84"/>
+      <c r="D18" s="85"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="27"/>
-      <c r="B19" s="29"/>
-      <c r="C19" s="29"/>
-      <c r="D19" s="36"/>
+      <c r="A19" s="15"/>
+      <c r="B19" s="17"/>
+      <c r="C19" s="17"/>
+      <c r="D19" s="24"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="83"/>
-      <c r="B20" s="29"/>
-      <c r="C20" s="29"/>
-      <c r="D20" s="128"/>
+      <c r="A20" s="37"/>
+      <c r="B20" s="17"/>
+      <c r="C20" s="17"/>
+      <c r="D20" s="67"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="27"/>
-      <c r="B21" s="29"/>
-      <c r="C21" s="29"/>
-      <c r="D21" s="36"/>
+      <c r="A21" s="15"/>
+      <c r="B21" s="17"/>
+      <c r="C21" s="17"/>
+      <c r="D21" s="24"/>
     </row>
     <row r="22" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="62"/>
-      <c r="B22" s="22"/>
-      <c r="C22" s="33"/>
-      <c r="D22" s="37"/>
+      <c r="A22" s="89"/>
+      <c r="B22" s="90"/>
+      <c r="C22" s="21"/>
+      <c r="D22" s="25"/>
     </row>
     <row r="23" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="55" t="s">
+      <c r="A23" s="83" t="s">
         <v>38</v>
       </c>
-      <c r="B23" s="57"/>
-      <c r="C23" s="57"/>
-      <c r="D23" s="56"/>
+      <c r="B23" s="84"/>
+      <c r="C23" s="84"/>
+      <c r="D23" s="85"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="27"/>
-      <c r="B24" s="29"/>
-      <c r="C24" s="29"/>
-      <c r="D24" s="36"/>
+      <c r="A24" s="15"/>
+      <c r="B24" s="17"/>
+      <c r="C24" s="17"/>
+      <c r="D24" s="24"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="83"/>
-      <c r="B25" s="29"/>
-      <c r="C25" s="29"/>
-      <c r="D25" s="128"/>
+      <c r="A25" s="37"/>
+      <c r="B25" s="17"/>
+      <c r="C25" s="17"/>
+      <c r="D25" s="67"/>
     </row>
     <row r="26" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="27"/>
-      <c r="B26" s="29"/>
-      <c r="C26" s="29"/>
-      <c r="D26" s="36"/>
+      <c r="A26" s="15"/>
+      <c r="B26" s="17"/>
+      <c r="C26" s="17"/>
+      <c r="D26" s="24"/>
     </row>
     <row r="27" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="55" t="s">
+      <c r="A27" s="83" t="s">
         <v>31</v>
       </c>
-      <c r="B27" s="57"/>
-      <c r="C27" s="57"/>
-      <c r="D27" s="56"/>
+      <c r="B27" s="84"/>
+      <c r="C27" s="84"/>
+      <c r="D27" s="85"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="26"/>
-      <c r="B28" s="34"/>
-      <c r="C28" s="34"/>
-      <c r="D28" s="35"/>
+      <c r="A28" s="14"/>
+      <c r="B28" s="22"/>
+      <c r="C28" s="22"/>
+      <c r="D28" s="23"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="83"/>
-      <c r="B29" s="29"/>
-      <c r="C29" s="29"/>
-      <c r="D29" s="128"/>
+      <c r="A29" s="37"/>
+      <c r="B29" s="17"/>
+      <c r="C29" s="17"/>
+      <c r="D29" s="67"/>
     </row>
     <row r="30" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="28"/>
-      <c r="B30" s="33"/>
-      <c r="C30" s="33"/>
-      <c r="D30" s="37"/>
+      <c r="A30" s="16"/>
+      <c r="B30" s="21"/>
+      <c r="C30" s="21"/>
+      <c r="D30" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="A27:D27"/>
-    <mergeCell ref="A11:D11"/>
-    <mergeCell ref="A13:D13"/>
-    <mergeCell ref="A14:D14"/>
-    <mergeCell ref="A18:D18"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A23:D23"/>
-    <mergeCell ref="C4:D5"/>
-    <mergeCell ref="F4:H4"/>
-    <mergeCell ref="F5:H5"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="F6:H6"/>
     <mergeCell ref="A7:D7"/>
     <mergeCell ref="E7:H7"/>
     <mergeCell ref="A1:H1"/>
@@ -22159,6 +22100,18 @@
     <mergeCell ref="E2:H2"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="F3:H3"/>
+    <mergeCell ref="C4:D5"/>
+    <mergeCell ref="F4:H4"/>
+    <mergeCell ref="F5:H5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="F6:H6"/>
+    <mergeCell ref="A27:D27"/>
+    <mergeCell ref="A11:D11"/>
+    <mergeCell ref="A13:D13"/>
+    <mergeCell ref="A14:D14"/>
+    <mergeCell ref="A18:D18"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A23:D23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -22182,26 +22135,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="131" t="s">
+      <c r="A1" s="109" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="131"/>
-      <c r="C1" s="131"/>
-      <c r="D1" s="131"/>
-      <c r="E1" s="131"/>
-      <c r="F1" s="131"/>
-      <c r="G1" s="131"/>
-      <c r="H1" s="131"/>
+      <c r="B1" s="109"/>
+      <c r="C1" s="109"/>
+      <c r="D1" s="109"/>
+      <c r="E1" s="109"/>
+      <c r="F1" s="109"/>
+      <c r="G1" s="109"/>
+      <c r="H1" s="109"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="55" t="s">
+      <c r="A2" s="83" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="56"/>
-      <c r="C2" s="55" t="s">
+      <c r="B2" s="85"/>
+      <c r="C2" s="83" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="56"/>
+      <c r="D2" s="85"/>
     </row>
     <row r="3" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
@@ -22210,295 +22163,290 @@
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="81" t="s">
+      <c r="C3" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="20" t="s">
+      <c r="D3" s="13" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="26">
+      <c r="A4" s="14">
         <v>1</v>
       </c>
-      <c r="B4" s="30">
+      <c r="B4" s="18">
         <v>8.44</v>
       </c>
-      <c r="C4" s="82"/>
-      <c r="D4" s="87" t="s">
+      <c r="C4" s="36"/>
+      <c r="D4" s="39" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="27">
+      <c r="A5" s="15">
         <v>2</v>
       </c>
-      <c r="B5" s="31">
+      <c r="B5" s="19">
         <v>8.44</v>
       </c>
-      <c r="C5" s="83"/>
-      <c r="D5" s="88" t="s">
+      <c r="C5" s="37"/>
+      <c r="D5" s="40" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="27">
+      <c r="A6" s="15">
         <v>3</v>
       </c>
-      <c r="B6" s="29">
+      <c r="B6" s="17">
         <v>8.0500000000000007</v>
       </c>
-      <c r="C6" s="83" t="s">
+      <c r="C6" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="88" t="s">
+      <c r="D6" s="40" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="27">
+      <c r="A7" s="15">
         <v>4</v>
       </c>
-      <c r="B7" s="29">
+      <c r="B7" s="17">
         <v>8.17</v>
       </c>
-      <c r="C7" s="84"/>
-      <c r="D7" s="92" t="s">
+      <c r="C7" s="38"/>
+      <c r="D7" s="42" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="27">
+      <c r="A8" s="15">
         <v>5</v>
       </c>
-      <c r="B8" s="32">
+      <c r="B8" s="20">
         <v>8.01</v>
       </c>
-      <c r="C8" s="29"/>
-      <c r="D8" s="36"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="24"/>
     </row>
     <row r="9" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="27">
+      <c r="A9" s="15">
         <v>6</v>
       </c>
-      <c r="B9" s="32">
+      <c r="B9" s="20">
         <v>8.06</v>
       </c>
-      <c r="C9" s="81" t="s">
+      <c r="C9" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="D9" s="20" t="s">
+      <c r="D9" s="13" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="27">
+      <c r="A10" s="15">
         <v>7</v>
       </c>
-      <c r="B10" s="32">
+      <c r="B10" s="20">
         <v>8.02</v>
       </c>
-      <c r="C10" s="82"/>
-      <c r="D10" s="87">
+      <c r="C10" s="36"/>
+      <c r="D10" s="39">
         <v>0.05</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="27">
+      <c r="A11" s="15">
         <v>8</v>
       </c>
-      <c r="B11" s="32">
+      <c r="B11" s="20">
         <v>8.02</v>
       </c>
-      <c r="C11" s="85"/>
-      <c r="D11" s="90">
+      <c r="C11" s="105"/>
+      <c r="D11" s="107">
         <v>8.1669999999999998</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="27">
+      <c r="A12" s="15">
         <v>9</v>
       </c>
-      <c r="B12" s="32">
+      <c r="B12" s="20">
         <v>8.0500000000000007</v>
       </c>
-      <c r="C12" s="86"/>
-      <c r="D12" s="91"/>
+      <c r="C12" s="106"/>
+      <c r="D12" s="108"/>
     </row>
     <row r="13" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="28">
+      <c r="A13" s="16">
         <v>10</v>
       </c>
-      <c r="B13" s="33">
+      <c r="B13" s="21">
         <v>8.41</v>
       </c>
-      <c r="C13" s="84" t="s">
+      <c r="C13" s="38" t="s">
         <v>24</v>
       </c>
-      <c r="D13" s="89">
+      <c r="D13" s="41">
         <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="28"/>
-      <c r="B14" s="33">
+      <c r="A14" s="16"/>
+      <c r="B14" s="21">
         <f>AVERAGE(B4:B13)</f>
         <v>8.166999999999998</v>
       </c>
-      <c r="C14" s="29"/>
-      <c r="D14" s="36"/>
+      <c r="C14" s="17"/>
+      <c r="D14" s="24"/>
     </row>
     <row r="15" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="55" t="s">
+      <c r="A15" s="83" t="s">
         <v>27</v>
       </c>
-      <c r="B15" s="56"/>
-      <c r="C15" s="55" t="s">
+      <c r="B15" s="85"/>
+      <c r="C15" s="83" t="s">
         <v>28</v>
       </c>
-      <c r="D15" s="56"/>
+      <c r="D15" s="85"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="58"/>
-      <c r="B16" s="59"/>
-      <c r="C16" s="58">
+      <c r="A16" s="116"/>
+      <c r="B16" s="97"/>
+      <c r="C16" s="116">
         <v>0.05</v>
       </c>
-      <c r="D16" s="59"/>
+      <c r="D16" s="97"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="60"/>
-      <c r="B17" s="61"/>
-      <c r="C17" s="60">
+      <c r="A17" s="86"/>
+      <c r="B17" s="88"/>
+      <c r="C17" s="86">
         <v>8.1669999999999998</v>
       </c>
-      <c r="D17" s="61"/>
+      <c r="D17" s="88"/>
     </row>
     <row r="18" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="62" t="s">
+      <c r="A18" s="89" t="s">
         <v>24</v>
       </c>
-      <c r="B18" s="63"/>
-      <c r="C18" s="62">
+      <c r="B18" s="102"/>
+      <c r="C18" s="89">
         <v>10</v>
       </c>
-      <c r="D18" s="63"/>
+      <c r="D18" s="102"/>
     </row>
     <row r="19" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="93" t="s">
+      <c r="A19" s="110" t="s">
         <v>29</v>
       </c>
-      <c r="B19" s="94"/>
-      <c r="C19" s="94"/>
-      <c r="D19" s="95"/>
+      <c r="B19" s="111"/>
+      <c r="C19" s="111"/>
+      <c r="D19" s="112"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="96"/>
-      <c r="B20" s="97"/>
-      <c r="C20" s="97"/>
-      <c r="D20" s="98"/>
+      <c r="A20" s="43"/>
+      <c r="B20" s="44"/>
+      <c r="C20" s="44"/>
+      <c r="D20" s="45"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="96"/>
-      <c r="B21" s="97"/>
-      <c r="C21" s="97"/>
-      <c r="D21" s="98"/>
+      <c r="A21" s="43"/>
+      <c r="B21" s="44"/>
+      <c r="C21" s="44"/>
+      <c r="D21" s="45"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="96"/>
-      <c r="B22" s="97"/>
-      <c r="C22" s="97"/>
-      <c r="D22" s="98"/>
+      <c r="A22" s="43"/>
+      <c r="B22" s="44"/>
+      <c r="C22" s="44"/>
+      <c r="D22" s="45"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="99"/>
-      <c r="B23" s="100"/>
-      <c r="C23" s="100"/>
-      <c r="D23" s="101"/>
+      <c r="A23" s="46"/>
+      <c r="B23" s="47"/>
+      <c r="C23" s="47"/>
+      <c r="D23" s="48"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="102" t="s">
+      <c r="A24" s="113" t="s">
         <v>30</v>
       </c>
-      <c r="B24" s="103"/>
-      <c r="C24" s="103"/>
-      <c r="D24" s="104"/>
+      <c r="B24" s="114"/>
+      <c r="C24" s="114"/>
+      <c r="D24" s="115"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="105"/>
-      <c r="B25" s="106"/>
-      <c r="C25" s="106"/>
-      <c r="D25" s="107"/>
+      <c r="A25" s="49"/>
+      <c r="B25" s="50"/>
+      <c r="C25" s="50"/>
+      <c r="D25" s="51"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="96"/>
-      <c r="B26" s="97"/>
-      <c r="C26" s="97"/>
-      <c r="D26" s="98"/>
+      <c r="A26" s="43"/>
+      <c r="B26" s="44"/>
+      <c r="C26" s="44"/>
+      <c r="D26" s="45"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="96"/>
-      <c r="B27" s="97"/>
-      <c r="C27" s="97"/>
-      <c r="D27" s="98"/>
+      <c r="A27" s="43"/>
+      <c r="B27" s="44"/>
+      <c r="C27" s="44"/>
+      <c r="D27" s="45"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="96"/>
-      <c r="B28" s="97"/>
-      <c r="C28" s="97"/>
-      <c r="D28" s="98"/>
+      <c r="A28" s="43"/>
+      <c r="B28" s="44"/>
+      <c r="C28" s="44"/>
+      <c r="D28" s="45"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="99"/>
-      <c r="B29" s="100"/>
-      <c r="C29" s="100"/>
-      <c r="D29" s="101"/>
+      <c r="A29" s="46"/>
+      <c r="B29" s="47"/>
+      <c r="C29" s="47"/>
+      <c r="D29" s="48"/>
     </row>
     <row r="30" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="108"/>
-      <c r="B30" s="100"/>
-      <c r="C30" s="100"/>
-      <c r="D30" s="109"/>
+      <c r="A30" s="52"/>
+      <c r="B30" s="47"/>
+      <c r="C30" s="47"/>
+      <c r="D30" s="53"/>
     </row>
     <row r="31" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="93" t="s">
+      <c r="A31" s="110" t="s">
         <v>31</v>
       </c>
-      <c r="B31" s="94"/>
-      <c r="C31" s="94"/>
-      <c r="D31" s="95"/>
+      <c r="B31" s="111"/>
+      <c r="C31" s="111"/>
+      <c r="D31" s="112"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="110"/>
-      <c r="B32" s="111"/>
-      <c r="C32" s="111"/>
-      <c r="D32" s="112"/>
+      <c r="A32" s="54"/>
+      <c r="B32" s="55"/>
+      <c r="C32" s="55"/>
+      <c r="D32" s="56"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="108"/>
-      <c r="B33" s="100"/>
-      <c r="C33" s="100"/>
-      <c r="D33" s="109"/>
+      <c r="A33" s="52"/>
+      <c r="B33" s="47"/>
+      <c r="C33" s="47"/>
+      <c r="D33" s="53"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="108"/>
-      <c r="B34" s="100"/>
-      <c r="C34" s="100"/>
-      <c r="D34" s="109"/>
+      <c r="A34" s="52"/>
+      <c r="B34" s="47"/>
+      <c r="C34" s="47"/>
+      <c r="D34" s="53"/>
     </row>
     <row r="35" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="113"/>
-      <c r="B35" s="114"/>
-      <c r="C35" s="114"/>
-      <c r="D35" s="115"/>
+      <c r="A35" s="57"/>
+      <c r="B35" s="58"/>
+      <c r="C35" s="58"/>
+      <c r="D35" s="59"/>
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="C18:D18"/>
     <mergeCell ref="A19:D19"/>
     <mergeCell ref="A24:D24"/>
     <mergeCell ref="A31:D31"/>
@@ -22508,6 +22456,11 @@
     <mergeCell ref="C16:D16"/>
     <mergeCell ref="A17:B17"/>
     <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="C18:D18"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="C2:D2"/>
   </mergeCells>
@@ -22519,10 +22472,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G51"/>
+  <dimension ref="A1:H50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B2" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34:D34"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22538,15 +22491,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="138" t="s">
+      <c r="A1" s="76" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="139"/>
-      <c r="C1" s="139"/>
-      <c r="D1" s="139"/>
-      <c r="E1" s="139"/>
-      <c r="F1" s="139"/>
-      <c r="G1" s="137"/>
+      <c r="B1" s="77"/>
+      <c r="C1" s="77"/>
+      <c r="D1" s="77"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="77"/>
+      <c r="G1" s="75"/>
     </row>
     <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -22556,11 +22509,11 @@
         <v>10</v>
       </c>
       <c r="C2" s="1"/>
-      <c r="D2" s="129" t="s">
+      <c r="D2" s="68" t="s">
         <v>39</v>
       </c>
       <c r="E2" s="1"/>
-      <c r="F2" s="129" t="s">
+      <c r="F2" s="68" t="s">
         <v>40</v>
       </c>
       <c r="G2" s="1"/>
@@ -22569,24 +22522,24 @@
       <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3" s="135">
+      <c r="B3" s="73">
         <v>34.15</v>
       </c>
-      <c r="C3" s="136">
+      <c r="C3" s="74">
         <f>POWER(B3-34.17,2)</f>
         <v>4.0000000000012508E-4</v>
       </c>
-      <c r="D3" s="134">
+      <c r="D3" s="72">
         <v>12</v>
       </c>
-      <c r="E3" s="134">
+      <c r="E3" s="72">
         <f>POWER(D3-D13,2)</f>
         <v>4.622499999999994E-2</v>
       </c>
-      <c r="F3" s="134">
+      <c r="F3" s="72">
         <v>15.18</v>
       </c>
-      <c r="G3" s="140">
+      <c r="G3" s="78">
         <f>POWER(F3-F13,2)</f>
         <v>0.45968400000000109</v>
       </c>
@@ -22595,17 +22548,17 @@
       <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="B4" s="38">
+      <c r="B4" s="26">
         <v>34</v>
       </c>
       <c r="C4" s="6">
         <f>POWER(B4-34.17,2)</f>
         <v>2.8900000000000581E-2</v>
       </c>
-      <c r="D4" s="46">
+      <c r="D4" s="30">
         <v>11.95</v>
       </c>
-      <c r="E4" s="46">
+      <c r="E4" s="30">
         <f>POWER(D4-D13,2)</f>
         <v>7.0225000000000301E-2</v>
       </c>
@@ -22621,7 +22574,7 @@
       <c r="A5" s="1">
         <v>3</v>
       </c>
-      <c r="B5" s="132">
+      <c r="B5" s="70">
         <v>34.1</v>
       </c>
       <c r="C5" s="6">
@@ -22647,14 +22600,14 @@
       <c r="A6" s="1">
         <v>4</v>
       </c>
-      <c r="B6" s="132">
+      <c r="B6" s="70">
         <v>34.1</v>
       </c>
       <c r="C6" s="6">
         <f t="shared" ref="C6:C12" si="0">POWER(B6-34.17,2)</f>
         <v>4.9000000000000397E-3</v>
       </c>
-      <c r="D6" s="46">
+      <c r="D6" s="30">
         <v>12</v>
       </c>
       <c r="E6" s="6">
@@ -22664,7 +22617,7 @@
       <c r="F6" s="7">
         <v>15.85</v>
       </c>
-      <c r="G6" s="141">
+      <c r="G6" s="79">
         <f>POWER(F6-F13,2)</f>
         <v>6.4000000000014322E-5</v>
       </c>
@@ -22673,14 +22626,14 @@
       <c r="A7" s="1">
         <v>5</v>
       </c>
-      <c r="B7" s="132">
+      <c r="B7" s="70">
         <v>34.1</v>
       </c>
       <c r="C7" s="6">
         <f t="shared" si="0"/>
         <v>4.9000000000000397E-3</v>
       </c>
-      <c r="D7" s="46">
+      <c r="D7" s="30">
         <v>12</v>
       </c>
       <c r="E7" s="6">
@@ -22699,17 +22652,17 @@
       <c r="A8" s="1">
         <v>6</v>
       </c>
-      <c r="B8" s="132">
+      <c r="B8" s="70">
         <v>34.450000000000003</v>
       </c>
       <c r="C8" s="6">
         <f t="shared" si="0"/>
         <v>7.8400000000000636E-2</v>
       </c>
-      <c r="D8" s="46">
+      <c r="D8" s="30">
         <v>12.75</v>
       </c>
-      <c r="E8" s="46">
+      <c r="E8" s="30">
         <f>POWER(D8-D13,2)</f>
         <v>0.28622500000000017</v>
       </c>
@@ -22725,17 +22678,17 @@
       <c r="A9" s="1">
         <v>7</v>
       </c>
-      <c r="B9" s="132">
+      <c r="B9" s="70">
         <v>34.200000000000003</v>
       </c>
       <c r="C9" s="6">
         <f t="shared" si="0"/>
         <v>9.0000000000006817E-4</v>
       </c>
-      <c r="D9" s="46">
+      <c r="D9" s="30">
         <v>12.9</v>
       </c>
-      <c r="E9" s="46">
+      <c r="E9" s="30">
         <f>POWER(D9-D13,2)</f>
         <v>0.46922500000000067</v>
       </c>
@@ -22751,17 +22704,17 @@
       <c r="A10" s="1">
         <v>8</v>
       </c>
-      <c r="B10" s="132">
+      <c r="B10" s="70">
         <v>34.200000000000003</v>
       </c>
       <c r="C10" s="6">
         <f t="shared" si="0"/>
         <v>9.0000000000006817E-4</v>
       </c>
-      <c r="D10" s="46">
+      <c r="D10" s="30">
         <v>11.8</v>
       </c>
-      <c r="E10" s="46">
+      <c r="E10" s="30">
         <f>POWER(D10-D13,2)</f>
         <v>0.1722249999999993</v>
       </c>
@@ -22777,17 +22730,17 @@
       <c r="A11" s="1">
         <v>9</v>
       </c>
-      <c r="B11" s="132">
+      <c r="B11" s="70">
         <v>34.4</v>
       </c>
       <c r="C11" s="6">
         <f t="shared" si="0"/>
         <v>5.2899999999998559E-2</v>
       </c>
-      <c r="D11" s="46">
+      <c r="D11" s="30">
         <v>11.8</v>
       </c>
-      <c r="E11" s="46">
+      <c r="E11" s="30">
         <f>POWER(D11-D13,2)</f>
         <v>0.1722249999999993</v>
       </c>
@@ -22803,7 +22756,7 @@
       <c r="A12" s="1">
         <v>10</v>
       </c>
-      <c r="B12" s="133">
+      <c r="B12" s="71">
         <v>34</v>
       </c>
       <c r="C12" s="6">
@@ -22827,7 +22780,7 @@
     </row>
     <row r="13" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
-      <c r="B13" s="133">
+      <c r="B13" s="71">
         <f>AVERAGE(B3:B12)</f>
         <v>34.169999999999995</v>
       </c>
@@ -22844,304 +22797,381 @@
       <c r="G13" s="9"/>
     </row>
     <row r="14" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="130" t="s">
+      <c r="A14" s="69" t="s">
         <v>41</v>
       </c>
-      <c r="B14" s="148"/>
-      <c r="C14" s="149">
+      <c r="B14" s="80"/>
+      <c r="C14" s="81">
         <f>SUM(C3:C12)</f>
         <v>0.20600000000000074</v>
       </c>
-      <c r="D14" s="149">
+      <c r="D14" s="81">
         <f>SUM(E3:E12)</f>
         <v>1.8952499999999985</v>
       </c>
-      <c r="E14" s="149"/>
-      <c r="F14" s="149">
+      <c r="E14" s="81"/>
+      <c r="F14" s="81">
         <f>SUM(G3:G12)</f>
         <v>0.65576000000000156</v>
       </c>
-      <c r="G14" s="150"/>
+      <c r="G14" s="82"/>
     </row>
     <row r="15" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="93" t="s">
-        <v>46</v>
-      </c>
-      <c r="B15" s="94"/>
-      <c r="C15" s="94"/>
-      <c r="D15" s="95"/>
-      <c r="E15" s="93" t="s">
+      <c r="A15" s="110" t="s">
+        <v>45</v>
+      </c>
+      <c r="B15" s="111"/>
+      <c r="C15" s="111"/>
+      <c r="D15" s="112"/>
+      <c r="E15" s="110" t="s">
         <v>48</v>
       </c>
-      <c r="F15" s="94"/>
-      <c r="G15" s="95"/>
+      <c r="F15" s="111"/>
+      <c r="G15" s="112"/>
     </row>
     <row r="16" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="93" t="s">
+      <c r="A16" s="110" t="s">
         <v>29</v>
       </c>
-      <c r="B16" s="94"/>
-      <c r="C16" s="94"/>
-      <c r="D16" s="95"/>
-      <c r="E16" s="93" t="s">
+      <c r="B16" s="111"/>
+      <c r="C16" s="111"/>
+      <c r="D16" s="112"/>
+      <c r="E16" s="110" t="s">
         <v>29</v>
       </c>
-      <c r="F16" s="94"/>
-      <c r="G16" s="95"/>
+      <c r="F16" s="111"/>
+      <c r="G16" s="112"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="96"/>
-      <c r="B17" s="97"/>
-      <c r="C17" s="100"/>
-      <c r="D17" s="101"/>
-      <c r="E17" s="96"/>
-      <c r="F17" s="97"/>
-      <c r="G17" s="101"/>
+      <c r="A17" s="43"/>
+      <c r="B17" s="44"/>
+      <c r="C17" s="47"/>
+      <c r="D17" s="48"/>
+      <c r="E17" s="43"/>
+      <c r="F17" s="44"/>
+      <c r="G17" s="48"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="96"/>
-      <c r="B18" s="97"/>
-      <c r="C18" s="100"/>
-      <c r="D18" s="101"/>
-      <c r="E18" s="96"/>
-      <c r="F18" s="97"/>
-      <c r="G18" s="101"/>
+      <c r="A18" s="43"/>
+      <c r="B18" s="44"/>
+      <c r="C18" s="47"/>
+      <c r="D18" s="48"/>
+      <c r="E18" s="43"/>
+      <c r="F18" s="44"/>
+      <c r="G18" s="48"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="96"/>
-      <c r="B19" s="97"/>
-      <c r="C19" s="100"/>
-      <c r="D19" s="101"/>
-      <c r="E19" s="96"/>
-      <c r="F19" s="97"/>
-      <c r="G19" s="101"/>
+      <c r="A19" s="43"/>
+      <c r="B19" s="44"/>
+      <c r="C19" s="47"/>
+      <c r="D19" s="48"/>
+      <c r="E19" s="43"/>
+      <c r="F19" s="44"/>
+      <c r="G19" s="48"/>
     </row>
     <row r="20" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="99"/>
-      <c r="B20" s="100"/>
-      <c r="C20" s="100"/>
-      <c r="D20" s="101"/>
-      <c r="E20" s="99"/>
-      <c r="F20" s="100"/>
-      <c r="G20" s="101"/>
+      <c r="A20" s="46"/>
+      <c r="B20" s="47"/>
+      <c r="C20" s="47"/>
+      <c r="D20" s="48"/>
+      <c r="E20" s="46"/>
+      <c r="F20" s="47"/>
+      <c r="G20" s="48"/>
     </row>
     <row r="21" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="93" t="s">
+      <c r="A21" s="110" t="s">
         <v>30</v>
       </c>
-      <c r="B21" s="94"/>
-      <c r="C21" s="94"/>
-      <c r="D21" s="95"/>
-      <c r="E21" s="93" t="s">
+      <c r="B21" s="111"/>
+      <c r="C21" s="111"/>
+      <c r="D21" s="112"/>
+      <c r="E21" s="110" t="s">
         <v>30</v>
       </c>
-      <c r="F21" s="94"/>
-      <c r="G21" s="95"/>
+      <c r="F21" s="111"/>
+      <c r="G21" s="112"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="96"/>
-      <c r="B22" s="97"/>
-      <c r="C22" s="100"/>
-      <c r="D22" s="101"/>
-      <c r="E22" s="96"/>
-      <c r="F22" s="97"/>
-      <c r="G22" s="101"/>
+      <c r="A22" s="43"/>
+      <c r="B22" s="44"/>
+      <c r="C22" s="47"/>
+      <c r="D22" s="48"/>
+      <c r="E22" s="43"/>
+      <c r="F22" s="44"/>
+      <c r="G22" s="48"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="96"/>
-      <c r="B23" s="97"/>
-      <c r="C23" s="100"/>
-      <c r="D23" s="101"/>
-      <c r="E23" s="96"/>
-      <c r="F23" s="97"/>
-      <c r="G23" s="101"/>
+      <c r="A23" s="43"/>
+      <c r="B23" s="44"/>
+      <c r="C23" s="47"/>
+      <c r="D23" s="48"/>
+      <c r="E23" s="43"/>
+      <c r="F23" s="44"/>
+      <c r="G23" s="48"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="96"/>
-      <c r="B24" s="97"/>
-      <c r="C24" s="100"/>
-      <c r="D24" s="101"/>
-      <c r="E24" s="96"/>
-      <c r="F24" s="97"/>
-      <c r="G24" s="101"/>
+      <c r="A24" s="43"/>
+      <c r="B24" s="44"/>
+      <c r="C24" s="47"/>
+      <c r="D24" s="48"/>
+      <c r="E24" s="43"/>
+      <c r="F24" s="44"/>
+      <c r="G24" s="48"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="96"/>
-      <c r="B25" s="97"/>
-      <c r="C25" s="100"/>
-      <c r="D25" s="101"/>
-      <c r="E25" s="96"/>
-      <c r="F25" s="97"/>
-      <c r="G25" s="101"/>
+      <c r="A25" s="43"/>
+      <c r="B25" s="44"/>
+      <c r="C25" s="47"/>
+      <c r="D25" s="48"/>
+      <c r="E25" s="43"/>
+      <c r="F25" s="44"/>
+      <c r="G25" s="48"/>
     </row>
     <row r="26" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="99"/>
-      <c r="B26" s="100"/>
-      <c r="C26" s="100"/>
-      <c r="D26" s="101"/>
-      <c r="E26" s="99"/>
-      <c r="F26" s="100"/>
-      <c r="G26" s="101"/>
+      <c r="A26" s="46"/>
+      <c r="B26" s="47"/>
+      <c r="C26" s="47"/>
+      <c r="D26" s="48"/>
+      <c r="E26" s="46"/>
+      <c r="F26" s="47"/>
+      <c r="G26" s="48"/>
     </row>
     <row r="27" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="93" t="s">
+      <c r="A27" s="110" t="s">
+        <v>46</v>
+      </c>
+      <c r="B27" s="111"/>
+      <c r="C27" s="111"/>
+      <c r="D27" s="112"/>
+      <c r="E27" s="110" t="s">
         <v>47</v>
       </c>
-      <c r="B27" s="94"/>
-      <c r="C27" s="94"/>
-      <c r="D27" s="95"/>
-      <c r="E27" s="93" t="s">
-        <v>49</v>
-      </c>
-      <c r="F27" s="94"/>
-      <c r="G27" s="95"/>
+      <c r="F27" s="111"/>
+      <c r="G27" s="112"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="99"/>
-      <c r="B28" s="100"/>
-      <c r="C28" s="100"/>
-      <c r="D28" s="101"/>
-      <c r="E28" s="99"/>
-      <c r="F28" s="100"/>
-      <c r="G28" s="101"/>
+      <c r="A28" s="46"/>
+      <c r="B28" s="47"/>
+      <c r="C28" s="47"/>
+      <c r="D28" s="48"/>
+      <c r="E28" s="46"/>
+      <c r="F28" s="47"/>
+      <c r="G28" s="48"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="108"/>
-      <c r="B29" s="100"/>
-      <c r="C29" s="100"/>
-      <c r="D29" s="101"/>
-      <c r="E29" s="108"/>
-      <c r="F29" s="100"/>
-      <c r="G29" s="101"/>
+      <c r="A29" s="52"/>
+      <c r="B29" s="47"/>
+      <c r="C29" s="47"/>
+      <c r="D29" s="48"/>
+      <c r="E29" s="52"/>
+      <c r="F29" s="47"/>
+      <c r="G29" s="48"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="108"/>
-      <c r="B30" s="100"/>
-      <c r="C30" s="100"/>
-      <c r="D30" s="101"/>
-      <c r="E30" s="108"/>
-      <c r="F30" s="100"/>
-      <c r="G30" s="101"/>
+      <c r="A30" s="52"/>
+      <c r="B30" s="47"/>
+      <c r="C30" s="47"/>
+      <c r="D30" s="48"/>
+      <c r="E30" s="52"/>
+      <c r="F30" s="47"/>
+      <c r="G30" s="48"/>
     </row>
     <row r="31" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="113"/>
-      <c r="B31" s="114"/>
-      <c r="C31" s="114"/>
-      <c r="D31" s="115"/>
-      <c r="E31" s="113"/>
-      <c r="F31" s="114"/>
-      <c r="G31" s="115"/>
+      <c r="A31" s="46"/>
+      <c r="B31" s="47"/>
+      <c r="C31" s="47"/>
+      <c r="D31" s="48"/>
+      <c r="E31" s="46"/>
+      <c r="F31" s="47"/>
+      <c r="G31" s="48"/>
     </row>
     <row r="32" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="58" t="s">
+      <c r="A32" s="110"/>
+      <c r="B32" s="111"/>
+      <c r="C32" s="111"/>
+      <c r="D32" s="111"/>
+      <c r="E32" s="111"/>
+      <c r="F32" s="111"/>
+      <c r="G32" s="112"/>
+    </row>
+    <row r="33" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="110" t="s">
+        <v>49</v>
+      </c>
+      <c r="B33" s="111"/>
+      <c r="C33" s="111"/>
+      <c r="D33" s="112"/>
+      <c r="E33" s="129" t="s">
+        <v>27</v>
+      </c>
+      <c r="F33" s="111" t="s">
+        <v>28</v>
+      </c>
+      <c r="G33" s="112"/>
+      <c r="H33" s="128"/>
+    </row>
+    <row r="34" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="110" t="s">
+        <v>29</v>
+      </c>
+      <c r="B34" s="111"/>
+      <c r="C34" s="111"/>
+      <c r="D34" s="112"/>
+      <c r="E34" s="133"/>
+      <c r="F34" s="131">
+        <v>0.05</v>
+      </c>
+      <c r="G34" s="132"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" s="43"/>
+      <c r="B35" s="44"/>
+      <c r="C35" s="47"/>
+      <c r="D35" s="48"/>
+      <c r="E35" s="130"/>
+      <c r="F35" s="17"/>
+      <c r="G35" s="17"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" s="43"/>
+      <c r="B36" s="44"/>
+      <c r="C36" s="47"/>
+      <c r="D36" s="48"/>
+      <c r="E36" s="17"/>
+      <c r="F36" s="17"/>
+      <c r="G36" s="17"/>
+    </row>
+    <row r="37" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="43"/>
+      <c r="B37" s="44"/>
+      <c r="C37" s="47"/>
+      <c r="D37" s="48"/>
+      <c r="E37" s="17"/>
+      <c r="F37" s="17"/>
+      <c r="G37" s="17"/>
+    </row>
+    <row r="38" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="110" t="s">
+        <v>30</v>
+      </c>
+      <c r="B38" s="111"/>
+      <c r="C38" s="111"/>
+      <c r="D38" s="112"/>
+      <c r="E38" s="17"/>
+      <c r="F38" s="17"/>
+      <c r="G38" s="17"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" s="43"/>
+      <c r="B39" s="44"/>
+      <c r="C39" s="47"/>
+      <c r="D39" s="48"/>
+      <c r="E39" s="17"/>
+      <c r="F39" s="17"/>
+      <c r="G39" s="17"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" s="43"/>
+      <c r="B40" s="44"/>
+      <c r="C40" s="47"/>
+      <c r="D40" s="48"/>
+      <c r="E40" s="17"/>
+      <c r="F40" s="17"/>
+      <c r="G40" s="17"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" s="43"/>
+      <c r="B41" s="44"/>
+      <c r="C41" s="47"/>
+      <c r="D41" s="48"/>
+      <c r="E41" s="17"/>
+      <c r="F41" s="17"/>
+      <c r="G41" s="17"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" s="43"/>
+      <c r="B42" s="44"/>
+      <c r="C42" s="47"/>
+      <c r="D42" s="48"/>
+      <c r="E42" s="17"/>
+      <c r="F42" s="17"/>
+      <c r="G42" s="17"/>
+    </row>
+    <row r="43" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="46"/>
+      <c r="B43" s="47"/>
+      <c r="C43" s="47"/>
+      <c r="D43" s="48"/>
+      <c r="E43" s="17"/>
+      <c r="F43" s="17"/>
+      <c r="G43" s="17"/>
+    </row>
+    <row r="44" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="110" t="s">
         <v>44</v>
       </c>
-      <c r="B32" s="19"/>
-      <c r="C32" s="19"/>
-      <c r="D32" s="19"/>
+      <c r="B44" s="111"/>
+      <c r="C44" s="111"/>
+      <c r="D44" s="112"/>
+      <c r="E44" s="17"/>
+      <c r="F44" s="17"/>
+      <c r="G44" s="17"/>
     </row>
-    <row r="33" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="55" t="s">
-        <v>27</v>
-      </c>
-      <c r="B33" s="56"/>
-      <c r="C33" s="60" t="s">
-        <v>28</v>
-      </c>
-      <c r="D33" s="18"/>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" s="46"/>
+      <c r="B45" s="47"/>
+      <c r="C45" s="47"/>
+      <c r="D45" s="48"/>
+      <c r="E45" s="17"/>
+      <c r="F45" s="17"/>
+      <c r="G45" s="17"/>
     </row>
-    <row r="34" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="55"/>
-      <c r="B34" s="56"/>
-      <c r="C34" s="60">
-        <v>0.05</v>
-      </c>
-      <c r="D34" s="61"/>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" s="52"/>
+      <c r="B46" s="47"/>
+      <c r="C46" s="47"/>
+      <c r="D46" s="48"/>
+      <c r="E46" s="17"/>
+      <c r="F46" s="17"/>
+      <c r="G46" s="17"/>
     </row>
-    <row r="35" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="146" t="s">
-        <v>29</v>
-      </c>
-      <c r="B35" s="147"/>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47" s="52"/>
+      <c r="B47" s="47"/>
+      <c r="C47" s="47"/>
+      <c r="D47" s="48"/>
+      <c r="E47" s="17"/>
+      <c r="F47" s="17"/>
+      <c r="G47" s="17"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="64"/>
-      <c r="B36" s="65"/>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A48" s="46"/>
+      <c r="B48" s="47"/>
+      <c r="C48" s="47"/>
+      <c r="D48" s="48"/>
+      <c r="E48" s="17"/>
+      <c r="F48" s="17"/>
+      <c r="G48" s="17"/>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="64"/>
-      <c r="B37" s="65"/>
+    <row r="49" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="16"/>
+      <c r="B49" s="21"/>
+      <c r="C49" s="21"/>
+      <c r="D49" s="25"/>
+      <c r="E49" s="17"/>
+      <c r="F49" s="17"/>
+      <c r="G49" s="17"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="64"/>
-      <c r="B38" s="65"/>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="66"/>
-      <c r="B39" s="67"/>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="144" t="s">
-        <v>30</v>
-      </c>
-      <c r="B40" s="145"/>
-      <c r="C40" s="145"/>
-      <c r="D40" s="145"/>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="68"/>
-      <c r="B41" s="69"/>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="70"/>
-      <c r="B42" s="71"/>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="70"/>
-      <c r="B43" s="71"/>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="70"/>
-      <c r="B44" s="71"/>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="72"/>
-      <c r="B45" s="73"/>
-    </row>
-    <row r="46" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="74"/>
-      <c r="B46" s="73"/>
-    </row>
-    <row r="47" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="142" t="s">
-        <v>45</v>
-      </c>
-      <c r="B47" s="143"/>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="75"/>
-      <c r="B48" s="76"/>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="77"/>
-      <c r="B49" s="78"/>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" s="77"/>
-      <c r="B50" s="78"/>
-    </row>
-    <row r="51" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="79"/>
-      <c r="B51" s="80"/>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E50" s="17"/>
+      <c r="F50" s="17"/>
+      <c r="G50" s="17"/>
     </row>
   </sheetData>
-  <mergeCells count="14">
-    <mergeCell ref="A32:D32"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="A40:D40"/>
+  <mergeCells count="15">
+    <mergeCell ref="A44:D44"/>
+    <mergeCell ref="F34:G34"/>
+    <mergeCell ref="A38:D38"/>
     <mergeCell ref="A21:D21"/>
     <mergeCell ref="E21:G21"/>
     <mergeCell ref="E15:G15"/>
@@ -23150,6 +23180,10 @@
     <mergeCell ref="A15:D15"/>
     <mergeCell ref="A16:D16"/>
     <mergeCell ref="A27:D27"/>
+    <mergeCell ref="A34:D34"/>
+    <mergeCell ref="F33:G33"/>
+    <mergeCell ref="A32:G32"/>
+    <mergeCell ref="A33:D33"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -23176,20 +23210,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="117" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
+      <c r="B1" s="117"/>
+      <c r="C1" s="117"/>
+      <c r="D1" s="117"/>
+      <c r="E1" s="117"/>
     </row>
     <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="24"/>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
+      <c r="A2" s="118"/>
+      <c r="B2" s="118"/>
+      <c r="C2" s="118"/>
+      <c r="D2" s="118"/>
+      <c r="E2" s="118"/>
     </row>
     <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
@@ -23215,9 +23249,9 @@
       <c r="B4" s="2">
         <v>8.44</v>
       </c>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="15"/>
+      <c r="C4" s="91"/>
+      <c r="D4" s="91"/>
+      <c r="E4" s="92"/>
     </row>
     <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
@@ -23226,9 +23260,9 @@
       <c r="B5" s="3">
         <v>8.44</v>
       </c>
-      <c r="C5" s="16"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="17"/>
+      <c r="C5" s="93"/>
+      <c r="D5" s="93"/>
+      <c r="E5" s="94"/>
     </row>
     <row r="6" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
@@ -23237,9 +23271,9 @@
       <c r="B6" s="4">
         <v>8.0500000000000007</v>
       </c>
-      <c r="C6" s="16"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="17"/>
+      <c r="C6" s="93"/>
+      <c r="D6" s="93"/>
+      <c r="E6" s="94"/>
     </row>
     <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
@@ -23248,9 +23282,9 @@
       <c r="B7" s="4">
         <v>8.17</v>
       </c>
-      <c r="C7" s="16"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="17"/>
+      <c r="C7" s="93"/>
+      <c r="D7" s="93"/>
+      <c r="E7" s="94"/>
     </row>
     <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
@@ -23259,9 +23293,9 @@
       <c r="B8" s="5">
         <v>8.01</v>
       </c>
-      <c r="C8" s="16"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="17"/>
+      <c r="C8" s="93"/>
+      <c r="D8" s="93"/>
+      <c r="E8" s="94"/>
     </row>
     <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
@@ -23270,9 +23304,9 @@
       <c r="B9" s="5">
         <v>8.06</v>
       </c>
-      <c r="C9" s="16"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="17"/>
+      <c r="C9" s="93"/>
+      <c r="D9" s="93"/>
+      <c r="E9" s="94"/>
     </row>
     <row r="10" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
@@ -23281,9 +23315,9 @@
       <c r="B10" s="5">
         <v>8.02</v>
       </c>
-      <c r="C10" s="16"/>
-      <c r="D10" s="16"/>
-      <c r="E10" s="17"/>
+      <c r="C10" s="93"/>
+      <c r="D10" s="93"/>
+      <c r="E10" s="94"/>
     </row>
     <row r="11" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
@@ -23292,9 +23326,9 @@
       <c r="B11" s="5">
         <v>8.02</v>
       </c>
-      <c r="C11" s="16"/>
-      <c r="D11" s="16"/>
-      <c r="E11" s="17"/>
+      <c r="C11" s="93"/>
+      <c r="D11" s="93"/>
+      <c r="E11" s="94"/>
     </row>
     <row r="12" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
@@ -23303,9 +23337,9 @@
       <c r="B12" s="5">
         <v>8.0500000000000007</v>
       </c>
-      <c r="C12" s="16"/>
-      <c r="D12" s="16"/>
-      <c r="E12" s="17"/>
+      <c r="C12" s="93"/>
+      <c r="D12" s="93"/>
+      <c r="E12" s="94"/>
     </row>
     <row r="13" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
@@ -23314,9 +23348,9 @@
       <c r="B13" s="4">
         <v>8.41</v>
       </c>
-      <c r="C13" s="16"/>
-      <c r="D13" s="16"/>
-      <c r="E13" s="17"/>
+      <c r="C13" s="93"/>
+      <c r="D13" s="93"/>
+      <c r="E13" s="94"/>
     </row>
     <row r="14" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
@@ -23341,8 +23375,8 @@
       <c r="C15" s="7">
         <v>0</v>
       </c>
-      <c r="D15" s="41"/>
-      <c r="E15" s="42"/>
+      <c r="D15" s="119"/>
+      <c r="E15" s="120"/>
     </row>
     <row r="16" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
@@ -23352,8 +23386,8 @@
       <c r="C16" s="7">
         <v>5.7999999999999996E-3</v>
       </c>
-      <c r="D16" s="43"/>
-      <c r="E16" s="44"/>
+      <c r="D16" s="121"/>
+      <c r="E16" s="122"/>
     </row>
     <row r="17" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
@@ -23363,7 +23397,7 @@
       <c r="C17" s="11">
         <v>5.7999999999999996E-3</v>
       </c>
-      <c r="D17" s="39" t="s">
+      <c r="D17" s="27" t="s">
         <v>13</v>
       </c>
       <c r="E17" s="12" t="s">
@@ -23371,24 +23405,24 @@
       </c>
     </row>
     <row r="18" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="48" t="s">
+      <c r="A18" s="123" t="s">
         <v>9</v>
       </c>
-      <c r="B18" s="25"/>
-      <c r="C18" s="25"/>
-      <c r="D18" s="25"/>
-      <c r="E18" s="25"/>
-      <c r="F18" s="25"/>
-      <c r="G18" s="49"/>
+      <c r="B18" s="124"/>
+      <c r="C18" s="124"/>
+      <c r="D18" s="124"/>
+      <c r="E18" s="124"/>
+      <c r="F18" s="124"/>
+      <c r="G18" s="125"/>
     </row>
     <row r="19" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="50"/>
-      <c r="B19" s="24"/>
-      <c r="C19" s="24"/>
-      <c r="D19" s="24"/>
-      <c r="E19" s="24"/>
-      <c r="F19" s="24"/>
-      <c r="G19" s="51"/>
+      <c r="A19" s="126"/>
+      <c r="B19" s="118"/>
+      <c r="C19" s="118"/>
+      <c r="D19" s="118"/>
+      <c r="E19" s="118"/>
+      <c r="F19" s="118"/>
+      <c r="G19" s="127"/>
     </row>
     <row r="20" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
@@ -23420,15 +23454,15 @@
       <c r="B21" s="2">
         <v>34.15</v>
       </c>
-      <c r="C21" s="45">
+      <c r="C21" s="29">
         <v>12</v>
       </c>
-      <c r="D21" s="45">
+      <c r="D21" s="29">
         <v>15.18</v>
       </c>
-      <c r="E21" s="14"/>
-      <c r="F21" s="14"/>
-      <c r="G21" s="15"/>
+      <c r="E21" s="91"/>
+      <c r="F21" s="91"/>
+      <c r="G21" s="92"/>
     </row>
     <row r="22" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
@@ -23437,15 +23471,15 @@
       <c r="B22" s="3">
         <v>34</v>
       </c>
-      <c r="C22" s="46">
+      <c r="C22" s="30">
         <v>11.95</v>
       </c>
       <c r="D22" s="7">
         <v>15.75</v>
       </c>
-      <c r="E22" s="16"/>
-      <c r="F22" s="16"/>
-      <c r="G22" s="17"/>
+      <c r="E22" s="93"/>
+      <c r="F22" s="93"/>
+      <c r="G22" s="94"/>
     </row>
     <row r="23" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
@@ -23460,9 +23494,9 @@
       <c r="D23" s="7">
         <v>15.8</v>
       </c>
-      <c r="E23" s="16"/>
-      <c r="F23" s="16"/>
-      <c r="G23" s="17"/>
+      <c r="E23" s="93"/>
+      <c r="F23" s="93"/>
+      <c r="G23" s="94"/>
     </row>
     <row r="24" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
@@ -23471,15 +23505,15 @@
       <c r="B24" s="5">
         <v>34.1</v>
       </c>
-      <c r="C24" s="46">
+      <c r="C24" s="30">
         <v>12</v>
       </c>
       <c r="D24" s="7">
         <v>15.85</v>
       </c>
-      <c r="E24" s="16"/>
-      <c r="F24" s="16"/>
-      <c r="G24" s="17"/>
+      <c r="E24" s="93"/>
+      <c r="F24" s="93"/>
+      <c r="G24" s="94"/>
     </row>
     <row r="25" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
@@ -23488,15 +23522,15 @@
       <c r="B25" s="5">
         <v>34.1</v>
       </c>
-      <c r="C25" s="46">
+      <c r="C25" s="30">
         <v>12</v>
       </c>
       <c r="D25" s="7">
         <v>15.8</v>
       </c>
-      <c r="E25" s="16"/>
-      <c r="F25" s="16"/>
-      <c r="G25" s="17"/>
+      <c r="E25" s="93"/>
+      <c r="F25" s="93"/>
+      <c r="G25" s="94"/>
     </row>
     <row r="26" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
@@ -23505,15 +23539,15 @@
       <c r="B26" s="5">
         <v>34.450000000000003</v>
       </c>
-      <c r="C26" s="46">
+      <c r="C26" s="30">
         <v>12.75</v>
       </c>
       <c r="D26" s="7">
         <v>16.100000000000001</v>
       </c>
-      <c r="E26" s="16"/>
-      <c r="F26" s="16"/>
-      <c r="G26" s="17"/>
+      <c r="E26" s="93"/>
+      <c r="F26" s="93"/>
+      <c r="G26" s="94"/>
     </row>
     <row r="27" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
@@ -23522,15 +23556,15 @@
       <c r="B27" s="5">
         <v>34.200000000000003</v>
       </c>
-      <c r="C27" s="46">
+      <c r="C27" s="30">
         <v>12.9</v>
       </c>
       <c r="D27" s="7">
         <v>16</v>
       </c>
-      <c r="E27" s="16"/>
-      <c r="F27" s="16"/>
-      <c r="G27" s="17"/>
+      <c r="E27" s="93"/>
+      <c r="F27" s="93"/>
+      <c r="G27" s="94"/>
     </row>
     <row r="28" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
@@ -23539,15 +23573,15 @@
       <c r="B28" s="5">
         <v>34.200000000000003</v>
       </c>
-      <c r="C28" s="46">
+      <c r="C28" s="30">
         <v>11.8</v>
       </c>
       <c r="D28" s="7">
         <v>16</v>
       </c>
-      <c r="E28" s="16"/>
-      <c r="F28" s="16"/>
-      <c r="G28" s="17"/>
+      <c r="E28" s="93"/>
+      <c r="F28" s="93"/>
+      <c r="G28" s="94"/>
     </row>
     <row r="29" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
@@ -23556,15 +23590,15 @@
       <c r="B29" s="5">
         <v>34.4</v>
       </c>
-      <c r="C29" s="46">
+      <c r="C29" s="30">
         <v>11.8</v>
       </c>
       <c r="D29" s="7">
         <v>16</v>
       </c>
-      <c r="E29" s="16"/>
-      <c r="F29" s="16"/>
-      <c r="G29" s="17"/>
+      <c r="E29" s="93"/>
+      <c r="F29" s="93"/>
+      <c r="G29" s="94"/>
     </row>
     <row r="30" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
@@ -23579,9 +23613,9 @@
       <c r="D30" s="7">
         <v>16.100000000000001</v>
       </c>
-      <c r="E30" s="16"/>
-      <c r="F30" s="16"/>
-      <c r="G30" s="17"/>
+      <c r="E30" s="93"/>
+      <c r="F30" s="93"/>
+      <c r="G30" s="94"/>
     </row>
     <row r="31" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="1"/>
@@ -23609,53 +23643,53 @@
     </row>
     <row r="32" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="1"/>
-      <c r="B32" s="47">
+      <c r="B32" s="31">
         <v>0.06</v>
       </c>
-      <c r="C32" s="46">
+      <c r="C32" s="30">
         <v>0.86</v>
       </c>
-      <c r="D32" s="46">
+      <c r="D32" s="30">
         <v>2.1999999999999999E-2</v>
       </c>
-      <c r="E32" s="46">
+      <c r="E32" s="30">
         <v>0</v>
       </c>
-      <c r="F32" s="16"/>
-      <c r="G32" s="17"/>
+      <c r="F32" s="93"/>
+      <c r="G32" s="94"/>
     </row>
     <row r="33" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="1"/>
-      <c r="B33" s="47">
+      <c r="B33" s="31">
         <v>2.9000000000000001E-2</v>
       </c>
-      <c r="C33" s="46">
+      <c r="C33" s="30">
         <v>2.9000000000000001E-2</v>
       </c>
-      <c r="D33" s="46">
+      <c r="D33" s="30">
         <v>2.9000000000000001E-2</v>
       </c>
-      <c r="E33" s="46">
+      <c r="E33" s="30">
         <v>5.7999999999999996E-3</v>
       </c>
-      <c r="F33" s="16"/>
-      <c r="G33" s="17"/>
+      <c r="F33" s="93"/>
+      <c r="G33" s="94"/>
     </row>
     <row r="34" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="1"/>
-      <c r="B34" s="52">
+      <c r="B34" s="32">
         <v>6.7000000000000004E-2</v>
       </c>
-      <c r="C34" s="53">
+      <c r="C34" s="33">
         <v>9.0800000000000006E-2</v>
       </c>
-      <c r="D34" s="53">
+      <c r="D34" s="33">
         <v>3.6999999999999998E-2</v>
       </c>
-      <c r="E34" s="53">
+      <c r="E34" s="33">
         <v>5.7999999999999996E-3</v>
       </c>
-      <c r="F34" s="54" t="s">
+      <c r="F34" s="34" t="s">
         <v>14</v>
       </c>
       <c r="G34" s="12" t="s">

</xml_diff>